<commit_message>
UPD web calc testing
</commit_message>
<xml_diff>
--- a/test_scenarios_calc/test_web_calc_v2.xlsx
+++ b/test_scenarios_calc/test_web_calc_v2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="154">
   <si>
     <t>Сценарии тестирования веб-калькулятора деления</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>TS27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL Injection </t>
   </si>
   <si>
     <t>TС27.01</t>
@@ -466,13 +463,22 @@
     <t>TС28.02</t>
   </si>
   <si>
-    <t>TС28.03</t>
-  </si>
-  <si>
     <t>Производительность. Время отклика</t>
   </si>
   <si>
     <t>Время отклика сервера находится в допустимых требованиями пределах</t>
+  </si>
+  <si>
+    <t>TS12</t>
+  </si>
+  <si>
+    <t>Кроссбраузерность</t>
+  </si>
+  <si>
+    <t>TС12.01</t>
+  </si>
+  <si>
+    <t>Безопасность</t>
   </si>
 </sst>
 </file>
@@ -949,9 +955,6 @@
   </cellStyleXfs>
   <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1036,9 +1039,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1056,6 +1056,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1361,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,1061 +1384,1065 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="13" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="37" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="40"/>
+      <c r="F5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="41" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="23" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="33" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="25" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="25" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="23" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="25" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="23" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="23" t="s">
+      <c r="A20" s="1"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="23" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="23" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="23" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="23" t="s">
+      <c r="A24" s="3"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="25" t="s">
+      <c r="A25" s="3"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="19" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="23" t="s">
+      <c r="A27" s="3"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="24" t="s">
+      <c r="G27" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="23" t="s">
+      <c r="A28" s="3"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="24" t="s">
+      <c r="G28" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="23" t="s">
+      <c r="A29" s="3"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="23" t="s">
+      <c r="A30" s="3"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="23" t="s">
+      <c r="A31" s="3"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="G31" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="23" t="s">
+      <c r="A32" s="3"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="25" t="s">
+      <c r="A33" s="3"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G35" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="52" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="53" t="s">
+      <c r="G36" s="52" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="55" t="s">
         <v>133</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="C38" s="57" t="s">
+      <c r="D38" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="G38" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="H38" s="60" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="55"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="D39" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="F38" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="G38" s="53" t="s">
+      <c r="E39" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="H38" s="54" t="s">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="55" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="57"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F39" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="G39" s="53" t="s">
+      <c r="B41" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="B41" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="D41" s="57" t="s">
-        <v>145</v>
-      </c>
-      <c r="E41" s="56" t="s">
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="55"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="F41" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="G41" s="53" t="s">
+      <c r="D42" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" s="55"/>
+      <c r="F42" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" s="52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="57"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="D42" s="57" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E42" s="57"/>
-      <c r="F42" s="56" t="s">
+      <c r="B44" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G42" s="53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="57" t="s">
-        <v>149</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="C44" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D53" s="41" t="s">
+      <c r="D53" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="41" t="s">
+      <c r="E53" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="F53" s="41" t="s">
+      <c r="F53" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="G53" s="44" t="s">
+      <c r="G53" s="43" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E55" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F55" s="20" t="s">
+      <c r="F55" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="G55" s="45" t="s">
+      <c r="G55" s="44" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="25" t="s">
+      <c r="A56" s="3"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="26" t="s">
+      <c r="D56" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E56" s="26" t="s">
+      <c r="E56" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="F56" s="26" t="s">
+      <c r="F56" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G56" s="46" t="s">
+      <c r="G56" s="45" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E58" s="20" t="s">
+      <c r="E58" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F58" s="20" t="s">
+      <c r="F58" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G58" s="45" t="s">
+      <c r="G58" s="44" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="23" t="s">
+      <c r="A59" s="3"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F59" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G59" s="48" t="s">
+      <c r="G59" s="47" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="25" t="s">
+      <c r="A60" s="3"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D60" s="26" t="s">
+      <c r="D60" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E60" s="26" t="s">
+      <c r="E60" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="F60" s="26" t="s">
+      <c r="F60" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="G60" s="46" t="s">
+      <c r="G60" s="45" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
     </row>
     <row r="62" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="57" t="s">
+      <c r="A62" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="58" t="s">
+      <c r="B62" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="59" t="s">
+      <c r="C62" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="D62" s="60" t="s">
+      <c r="D62" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="41"/>
-      <c r="F62" s="49" t="s">
+      <c r="E62" s="40"/>
+      <c r="F62" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="G62" s="44" t="s">
+      <c r="G62" s="43" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4" t="s">
+      <c r="E64" s="3"/>
+      <c r="F64" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G64" s="47" t="s">
+      <c r="G64" s="46" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="50" t="s">
+      <c r="B66" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4" t="s">
+      <c r="E66" s="3"/>
+      <c r="F66" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G66" s="47" t="s">
+      <c r="G66" s="46" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>